<commit_message>
add main.py and fix Duke 2018 Mascot
</commit_message>
<xml_diff>
--- a/conferences.xlsx
+++ b/conferences.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/Bowl Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4D9470-143C-594A-AB86-673C236DBCBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509063E2-62A2-D641-BDA6-0E6DD8A05738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8040" yWindow="1820" windowWidth="27640" windowHeight="16940" xr2:uid="{3263E9AF-F9C0-DC44-AEF2-F5BCA61BF551}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="260">
   <si>
     <t>School</t>
   </si>
@@ -811,6 +811,9 @@
   </si>
   <si>
     <t>BIG 12</t>
+  </si>
+  <si>
+    <t>Blue Devils</t>
   </si>
 </sst>
 </file>
@@ -1172,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5BD186-F85F-7546-B82F-A6AAE7F38B00}">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="E237" sqref="E237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6111,7 +6114,7 @@
         <v>52</v>
       </c>
       <c r="B247" t="s">
-        <v>53</v>
+        <v>259</v>
       </c>
       <c r="C247">
         <v>2018</v>

</xml_diff>

<commit_message>
get descriptive stats on results and edit some issues in conferences.xlsx file
</commit_message>
<xml_diff>
--- a/conferences.xlsx
+++ b/conferences.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rspoonmore/Documents/Coding/CollegeFootballBowlGames/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509063E2-62A2-D641-BDA6-0E6DD8A05738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE93AF7E-A8BB-754C-A124-93F24BC88EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="1820" windowWidth="27640" windowHeight="16940" xr2:uid="{3263E9AF-F9C0-DC44-AEF2-F5BCA61BF551}"/>
+    <workbookView xWindow="9580" yWindow="2880" windowWidth="27640" windowHeight="16940" xr2:uid="{3263E9AF-F9C0-DC44-AEF2-F5BCA61BF551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$291</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$287</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="261">
   <si>
     <t>School</t>
   </si>
@@ -814,6 +814,9 @@
   </si>
   <si>
     <t>Blue Devils</t>
+  </si>
+  <si>
+    <t>Texas Tech</t>
   </si>
 </sst>
 </file>
@@ -1173,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C5BD186-F85F-7546-B82F-A6AAE7F38B00}">
-  <dimension ref="A1:F291"/>
+  <dimension ref="A1:F288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="E237" sqref="E237"/>
+    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
+      <selection activeCell="C288" sqref="C288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3291,7 +3294,7 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>189</v>
+        <v>260</v>
       </c>
       <c r="B106" t="s">
         <v>190</v>
@@ -5371,56 +5374,56 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="B210" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="C210">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D210" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="E210" t="s">
         <v>237</v>
       </c>
       <c r="F210" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>43</v>
+        <v>208</v>
       </c>
       <c r="B211" t="s">
-        <v>21</v>
+        <v>132</v>
       </c>
       <c r="C211">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D211" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="E211" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="F211" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>135</v>
+        <v>194</v>
       </c>
       <c r="B212" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="C212">
         <v>2018</v>
       </c>
       <c r="D212" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E212" t="s">
         <v>237</v>
@@ -5431,19 +5434,19 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>208</v>
+        <v>91</v>
       </c>
       <c r="B213" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="C213">
         <v>2018</v>
       </c>
       <c r="D213" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E213" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="F213" t="s">
         <v>248</v>
@@ -5451,36 +5454,36 @@
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>194</v>
+        <v>12</v>
       </c>
       <c r="B214" t="s">
-        <v>195</v>
+        <v>13</v>
       </c>
       <c r="C214">
         <v>2018</v>
       </c>
       <c r="D214" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E214" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F214" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B215" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="C215">
         <v>2018</v>
       </c>
       <c r="D215" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="E215" t="s">
         <v>237</v>
@@ -5491,39 +5494,39 @@
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="B216" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C216">
         <v>2018</v>
       </c>
       <c r="D216" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E216" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F216" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B217" t="s">
-        <v>66</v>
+        <v>29</v>
       </c>
       <c r="C217">
         <v>2018</v>
       </c>
       <c r="D217" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="E217" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F217" t="s">
         <v>248</v>
@@ -5531,19 +5534,19 @@
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>56</v>
+        <v>251</v>
       </c>
       <c r="B218" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C218">
         <v>2018</v>
       </c>
       <c r="D218" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E218" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F218" t="s">
         <v>248</v>
@@ -5551,16 +5554,16 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="B219" t="s">
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="C219">
         <v>2018</v>
       </c>
       <c r="D219" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E219" t="s">
         <v>235</v>
@@ -5571,19 +5574,19 @@
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>251</v>
+        <v>198</v>
       </c>
       <c r="B220" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="C220">
         <v>2018</v>
       </c>
       <c r="D220" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E220" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F220" t="s">
         <v>248</v>
@@ -5591,19 +5594,19 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>113</v>
+        <v>137</v>
       </c>
       <c r="B221" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="C221">
         <v>2018</v>
       </c>
       <c r="D221" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E221" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F221" t="s">
         <v>248</v>
@@ -5611,19 +5614,19 @@
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>198</v>
+        <v>141</v>
       </c>
       <c r="B222" t="s">
-        <v>199</v>
+        <v>142</v>
       </c>
       <c r="C222">
         <v>2018</v>
       </c>
       <c r="D222" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E222" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F222" t="s">
         <v>248</v>
@@ -5631,16 +5634,16 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="B223" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="C223">
         <v>2018</v>
       </c>
       <c r="D223" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E223" t="s">
         <v>237</v>
@@ -5651,16 +5654,16 @@
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="B224" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="C224">
         <v>2018</v>
       </c>
       <c r="D224" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="E224" t="s">
         <v>235</v>
@@ -5671,19 +5674,19 @@
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="B225" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
       <c r="C225">
         <v>2018</v>
       </c>
       <c r="D225" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="E225" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F225" t="s">
         <v>248</v>
@@ -5691,19 +5694,19 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>98</v>
+        <v>191</v>
       </c>
       <c r="B226" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
       <c r="C226">
         <v>2018</v>
       </c>
       <c r="D226" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E226" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F226" t="s">
         <v>248</v>
@@ -5711,16 +5714,16 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>174</v>
+        <v>57</v>
       </c>
       <c r="B227" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C227">
         <v>2018</v>
       </c>
       <c r="D227" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E227" t="s">
         <v>235</v>
@@ -5731,19 +5734,19 @@
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>191</v>
+        <v>33</v>
       </c>
       <c r="B228" t="s">
-        <v>192</v>
+        <v>34</v>
       </c>
       <c r="C228">
         <v>2018</v>
       </c>
-      <c r="D228" t="s">
-        <v>234</v>
+      <c r="D228" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="E228" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="F228" t="s">
         <v>248</v>
@@ -5751,19 +5754,19 @@
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>57</v>
+        <v>226</v>
       </c>
       <c r="B229" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C229">
         <v>2018</v>
       </c>
       <c r="D229" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="E229" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F229" t="s">
         <v>248</v>
@@ -5771,36 +5774,36 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>33</v>
+        <v>219</v>
       </c>
       <c r="B230" t="s">
-        <v>34</v>
+        <v>220</v>
       </c>
       <c r="C230">
         <v>2018</v>
       </c>
-      <c r="D230" s="1" t="s">
-        <v>241</v>
+      <c r="D230" t="s">
+        <v>243</v>
       </c>
       <c r="E230" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F230" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>226</v>
+        <v>104</v>
       </c>
       <c r="B231" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C231">
         <v>2018</v>
       </c>
       <c r="D231" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="E231" t="s">
         <v>237</v>
@@ -5811,30 +5814,30 @@
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>219</v>
+        <v>18</v>
       </c>
       <c r="B232" t="s">
-        <v>220</v>
+        <v>19</v>
       </c>
       <c r="C232">
         <v>2018</v>
       </c>
-      <c r="D232" t="s">
-        <v>243</v>
+      <c r="D232" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="E232" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F232" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="B233" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="C233">
         <v>2018</v>
@@ -5851,19 +5854,19 @@
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B234" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C234">
         <v>2018</v>
       </c>
-      <c r="D234" s="1" t="s">
-        <v>241</v>
+      <c r="D234" t="s">
+        <v>234</v>
       </c>
       <c r="E234" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="F234" t="s">
         <v>248</v>
@@ -5871,19 +5874,19 @@
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>74</v>
+        <v>193</v>
       </c>
       <c r="B235" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
       <c r="C235">
         <v>2018</v>
       </c>
       <c r="D235" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="E235" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F235" t="s">
         <v>248</v>
@@ -5891,19 +5894,19 @@
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B236" t="s">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="C236">
         <v>2018</v>
       </c>
       <c r="D236" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E236" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F236" t="s">
         <v>248</v>
@@ -5911,19 +5914,19 @@
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>193</v>
+        <v>93</v>
       </c>
       <c r="B237" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="C237">
         <v>2018</v>
       </c>
       <c r="D237" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E237" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F237" t="s">
         <v>248</v>
@@ -5931,39 +5934,39 @@
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B238" t="s">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C238">
         <v>2018</v>
       </c>
       <c r="D238" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E238" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="F238" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="B239" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="C239">
         <v>2018</v>
       </c>
       <c r="D239" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="E239" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F239" t="s">
         <v>248</v>
@@ -5971,19 +5974,19 @@
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="B240" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
       <c r="C240">
         <v>2018</v>
       </c>
       <c r="D240" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="E240" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="F240" t="s">
         <v>247</v>
@@ -5991,39 +5994,39 @@
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B241" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="C241">
         <v>2018</v>
       </c>
       <c r="D241" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E241" t="s">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="F241" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="242" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>115</v>
+        <v>181</v>
       </c>
       <c r="B242" t="s">
-        <v>116</v>
+        <v>182</v>
       </c>
       <c r="C242">
         <v>2018</v>
       </c>
       <c r="D242" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E242" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="F242" t="s">
         <v>247</v>
@@ -6031,19 +6034,19 @@
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>70</v>
+        <v>253</v>
       </c>
       <c r="B243" t="s">
-        <v>71</v>
+        <v>203</v>
       </c>
       <c r="C243">
         <v>2018</v>
       </c>
       <c r="D243" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E243" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F243" t="s">
         <v>247</v>
@@ -6051,39 +6054,39 @@
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B244" t="s">
-        <v>182</v>
+        <v>62</v>
       </c>
       <c r="C244">
         <v>2018</v>
       </c>
       <c r="D244" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="E244" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="F244" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>253</v>
+        <v>52</v>
       </c>
       <c r="B245" t="s">
-        <v>203</v>
+        <v>259</v>
       </c>
       <c r="C245">
         <v>2018</v>
       </c>
       <c r="D245" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E245" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="F245" t="s">
         <v>247</v>
@@ -6091,39 +6094,39 @@
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>183</v>
+        <v>105</v>
       </c>
       <c r="B246" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C246">
         <v>2018</v>
       </c>
       <c r="D246" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="E246" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F246" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>52</v>
+        <v>227</v>
       </c>
       <c r="B247" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
       <c r="C247">
         <v>2018</v>
       </c>
       <c r="D247" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="E247" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="F247" t="s">
         <v>247</v>
@@ -6131,19 +6134,19 @@
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>105</v>
+        <v>24</v>
       </c>
       <c r="B248" t="s">
-        <v>106</v>
+        <v>25</v>
       </c>
       <c r="C248">
         <v>2018</v>
       </c>
       <c r="D248" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="E248" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F248" t="s">
         <v>247</v>
@@ -6151,19 +6154,19 @@
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="B249" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="C249">
         <v>2018</v>
       </c>
       <c r="D249" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="E249" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F249" t="s">
         <v>247</v>
@@ -6171,19 +6174,19 @@
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B250" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C250">
         <v>2018</v>
       </c>
       <c r="D250" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="E250" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="F250" t="s">
         <v>247</v>
@@ -6191,19 +6194,19 @@
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>213</v>
+        <v>159</v>
       </c>
       <c r="B251" t="s">
-        <v>214</v>
+        <v>160</v>
       </c>
       <c r="C251">
         <v>2018</v>
       </c>
       <c r="D251" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="E251" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F251" t="s">
         <v>247</v>
@@ -6211,19 +6214,19 @@
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>20</v>
+        <v>223</v>
       </c>
       <c r="B252" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C252">
         <v>2018</v>
       </c>
       <c r="D252" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="E252" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="F252" t="s">
         <v>247</v>
@@ -6231,19 +6234,19 @@
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="B253" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="C253">
         <v>2018</v>
       </c>
       <c r="D253" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="E253" t="s">
-        <v>237</v>
+        <v>255</v>
       </c>
       <c r="F253" t="s">
         <v>247</v>
@@ -6251,10 +6254,10 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>223</v>
+        <v>81</v>
       </c>
       <c r="B254" t="s">
-        <v>9</v>
+        <v>82</v>
       </c>
       <c r="C254">
         <v>2018</v>
@@ -6271,19 +6274,19 @@
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>179</v>
+        <v>222</v>
       </c>
       <c r="B255" t="s">
-        <v>180</v>
+        <v>34</v>
       </c>
       <c r="C255">
         <v>2018</v>
       </c>
       <c r="D255" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E255" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="F255" t="s">
         <v>247</v>
@@ -6291,39 +6294,39 @@
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>81</v>
+        <v>139</v>
       </c>
       <c r="B256" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="C256">
         <v>2018</v>
       </c>
-      <c r="D256" t="s">
-        <v>258</v>
+      <c r="D256" s="1" t="s">
+        <v>241</v>
       </c>
       <c r="E256" t="s">
         <v>256</v>
       </c>
       <c r="F256" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>222</v>
+        <v>43</v>
       </c>
       <c r="B257" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C257">
         <v>2018</v>
       </c>
       <c r="D257" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E257" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="F257" t="s">
         <v>247</v>
@@ -6331,39 +6334,39 @@
     </row>
     <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>139</v>
+        <v>6</v>
       </c>
       <c r="B258" t="s">
-        <v>140</v>
+        <v>7</v>
       </c>
       <c r="C258">
         <v>2018</v>
       </c>
-      <c r="D258" s="1" t="s">
-        <v>241</v>
+      <c r="D258" t="s">
+        <v>236</v>
       </c>
       <c r="E258" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="F258" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
       <c r="B259" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="C259">
         <v>2018</v>
       </c>
       <c r="D259" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="E259" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="F259" t="s">
         <v>247</v>
@@ -6371,19 +6374,19 @@
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>6</v>
+        <v>109</v>
       </c>
       <c r="B260" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="C260">
         <v>2018</v>
       </c>
       <c r="D260" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="E260" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F260" t="s">
         <v>247</v>
@@ -6391,19 +6394,19 @@
     </row>
     <row r="261" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>145</v>
+        <v>59</v>
       </c>
       <c r="B261" t="s">
-        <v>146</v>
+        <v>60</v>
       </c>
       <c r="C261">
         <v>2018</v>
       </c>
       <c r="D261" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="E261" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="F261" t="s">
         <v>247</v>
@@ -6411,16 +6414,16 @@
     </row>
     <row r="262" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="B262" t="s">
-        <v>110</v>
+        <v>173</v>
       </c>
       <c r="C262">
         <v>2018</v>
       </c>
       <c r="D262" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="E262" t="s">
         <v>235</v>
@@ -6431,19 +6434,19 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>59</v>
+        <v>215</v>
       </c>
       <c r="B263" t="s">
-        <v>60</v>
+        <v>216</v>
       </c>
       <c r="C263">
         <v>2018</v>
       </c>
       <c r="D263" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E263" t="s">
-        <v>235</v>
+        <v>254</v>
       </c>
       <c r="F263" t="s">
         <v>247</v>
@@ -6451,59 +6454,59 @@
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>172</v>
+        <v>127</v>
       </c>
       <c r="B264" t="s">
-        <v>173</v>
+        <v>128</v>
       </c>
       <c r="C264">
         <v>2018</v>
       </c>
       <c r="D264" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E264" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F264" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>215</v>
+        <v>16</v>
       </c>
       <c r="B265" t="s">
-        <v>216</v>
+        <v>17</v>
       </c>
       <c r="C265">
         <v>2018</v>
       </c>
       <c r="D265" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="E265" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="F265" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="B266" t="s">
-        <v>128</v>
+        <v>42</v>
       </c>
       <c r="C266">
         <v>2018</v>
       </c>
       <c r="D266" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
       <c r="E266" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F266" t="s">
         <v>248</v>
@@ -6511,59 +6514,59 @@
     </row>
     <row r="267" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="B267" t="s">
-        <v>17</v>
+        <v>218</v>
       </c>
       <c r="C267">
         <v>2018</v>
       </c>
       <c r="D267" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="E267" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="F267" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="268" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="B268" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="C268">
         <v>2018</v>
       </c>
       <c r="D268" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="E268" t="s">
         <v>235</v>
       </c>
       <c r="F268" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>217</v>
+        <v>151</v>
       </c>
       <c r="B269" t="s">
-        <v>218</v>
+        <v>152</v>
       </c>
       <c r="C269">
         <v>2018</v>
       </c>
       <c r="D269" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E269" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F269" t="s">
         <v>247</v>
@@ -6571,16 +6574,16 @@
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B270" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C270">
         <v>2018</v>
       </c>
       <c r="D270" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="E270" t="s">
         <v>235</v>
@@ -6591,19 +6594,19 @@
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B271" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C271">
         <v>2018</v>
       </c>
       <c r="D271" t="s">
-        <v>239</v>
+        <v>258</v>
       </c>
       <c r="E271" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="F271" t="s">
         <v>247</v>
@@ -6611,19 +6614,19 @@
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="B272" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C272">
         <v>2018</v>
       </c>
       <c r="D272" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="E272" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F272" t="s">
         <v>247</v>
@@ -6631,19 +6634,19 @@
     </row>
     <row r="273" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>147</v>
+        <v>206</v>
       </c>
       <c r="B273" t="s">
-        <v>148</v>
+        <v>207</v>
       </c>
       <c r="C273">
         <v>2018</v>
       </c>
       <c r="D273" t="s">
-        <v>258</v>
+        <v>239</v>
       </c>
       <c r="E273" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="F273" t="s">
         <v>247</v>
@@ -6651,16 +6654,16 @@
     </row>
     <row r="274" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>138</v>
+        <v>188</v>
       </c>
       <c r="B274" t="s">
-        <v>11</v>
+        <v>132</v>
       </c>
       <c r="C274">
         <v>2018</v>
       </c>
       <c r="D274" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="E274" t="s">
         <v>237</v>
@@ -6671,19 +6674,19 @@
     </row>
     <row r="275" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>206</v>
+        <v>123</v>
       </c>
       <c r="B275" t="s">
-        <v>207</v>
+        <v>124</v>
       </c>
       <c r="C275">
         <v>2018</v>
       </c>
       <c r="D275" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="E275" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="F275" t="s">
         <v>247</v>
@@ -6691,19 +6694,19 @@
     </row>
     <row r="276" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>188</v>
+        <v>252</v>
       </c>
       <c r="B276" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="C276">
         <v>2018</v>
       </c>
       <c r="D276" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E276" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="F276" t="s">
         <v>247</v>
@@ -6711,19 +6714,19 @@
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>123</v>
+        <v>177</v>
       </c>
       <c r="B277" t="s">
-        <v>124</v>
+        <v>178</v>
       </c>
       <c r="C277">
         <v>2018</v>
       </c>
       <c r="D277" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E277" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="F277" t="s">
         <v>247</v>
@@ -6731,19 +6734,19 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>252</v>
+        <v>186</v>
       </c>
       <c r="B278" t="s">
-        <v>58</v>
+        <v>187</v>
       </c>
       <c r="C278">
         <v>2018</v>
       </c>
       <c r="D278" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="E278" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F278" t="s">
         <v>247</v>
@@ -6751,19 +6754,19 @@
     </row>
     <row r="279" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>177</v>
+        <v>67</v>
       </c>
       <c r="B279" t="s">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="C279">
         <v>2018</v>
       </c>
       <c r="D279" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E279" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="F279" t="s">
         <v>247</v>
@@ -6771,19 +6774,19 @@
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>186</v>
+        <v>97</v>
       </c>
       <c r="B280" t="s">
-        <v>187</v>
+        <v>21</v>
       </c>
       <c r="C280">
         <v>2018</v>
       </c>
       <c r="D280" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="E280" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="F280" t="s">
         <v>247</v>
@@ -6791,39 +6794,39 @@
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
       <c r="B281" t="s">
-        <v>66</v>
+        <v>201</v>
       </c>
       <c r="C281">
         <v>2018</v>
       </c>
       <c r="D281" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="E281" t="s">
         <v>235</v>
       </c>
       <c r="F281" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>97</v>
+        <v>143</v>
       </c>
       <c r="B282" t="s">
-        <v>21</v>
+        <v>144</v>
       </c>
       <c r="C282">
         <v>2018</v>
       </c>
       <c r="D282" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="E282" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F282" t="s">
         <v>247</v>
@@ -6831,39 +6834,39 @@
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="B283" t="s">
-        <v>201</v>
+        <v>51</v>
       </c>
       <c r="C283">
         <v>2018</v>
       </c>
       <c r="D283" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="E283" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="F283" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="B284" t="s">
-        <v>144</v>
+        <v>66</v>
       </c>
       <c r="C284">
         <v>2018</v>
       </c>
       <c r="D284" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="E284" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F284" t="s">
         <v>247</v>
@@ -6871,19 +6874,19 @@
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>221</v>
+        <v>79</v>
       </c>
       <c r="B285" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="C285">
         <v>2018</v>
       </c>
       <c r="D285" t="s">
-        <v>239</v>
+        <v>257</v>
       </c>
       <c r="E285" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="F285" t="s">
         <v>247</v>
@@ -6891,10 +6894,10 @@
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="B286" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="C286">
         <v>2018</v>
@@ -6903,7 +6906,7 @@
         <v>236</v>
       </c>
       <c r="E286" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F286" t="s">
         <v>247</v>
@@ -6911,10 +6914,10 @@
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="B287" t="s">
-        <v>80</v>
+        <v>156</v>
       </c>
       <c r="C287">
         <v>2018</v>
@@ -6923,7 +6926,7 @@
         <v>257</v>
       </c>
       <c r="E287" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F287" t="s">
         <v>247</v>
@@ -6931,82 +6934,22 @@
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B288" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="C288">
         <v>2018</v>
       </c>
       <c r="D288" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E288" t="s">
         <v>235</v>
       </c>
       <c r="F288" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A289" t="s">
-        <v>155</v>
-      </c>
-      <c r="B289" t="s">
-        <v>156</v>
-      </c>
-      <c r="C289">
-        <v>2018</v>
-      </c>
-      <c r="D289" t="s">
-        <v>257</v>
-      </c>
-      <c r="E289" t="s">
-        <v>235</v>
-      </c>
-      <c r="F289" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A290" t="s">
-        <v>43</v>
-      </c>
-      <c r="B290" t="s">
-        <v>21</v>
-      </c>
-      <c r="C290">
-        <v>2018</v>
-      </c>
-      <c r="D290" t="s">
-        <v>243</v>
-      </c>
-      <c r="E290" t="s">
-        <v>255</v>
-      </c>
-      <c r="F290" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A291" t="s">
-        <v>6</v>
-      </c>
-      <c r="B291" t="s">
-        <v>7</v>
-      </c>
-      <c r="C291">
-        <v>2018</v>
-      </c>
-      <c r="D291" t="s">
-        <v>236</v>
-      </c>
-      <c r="E291" t="s">
-        <v>237</v>
-      </c>
-      <c r="F291" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>